<commit_message>
Generar documentación Gastos Alumnos
</commit_message>
<xml_diff>
--- a/public/Anexo 6-Gastos_FCT_2DAW.xlsx
+++ b/public/Anexo 6-Gastos_FCT_2DAW.xlsx
@@ -115,7 +115,7 @@
     <t>Roldán Vara, Sergio</t>
   </si>
   <si>
-    <t>Rubio Baños, Joaquín José</t>
+    <t>Torres Gijón, Beatriz</t>
   </si>
   <si>
     <t>(1) Cuantía €/km según Instrucciones de la Viceconsejería de Educación, Universidades e Investigación vigentes</t>
@@ -685,7 +685,9 @@
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
-      <c r="K8"/>
+      <c r="K8">
+        <v>5047.0</v>
+      </c>
       <c r="L8"/>
       <c r="M8"/>
     </row>
@@ -702,7 +704,9 @@
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
-      <c r="K9"/>
+      <c r="K9">
+        <v>6.0</v>
+      </c>
       <c r="L9"/>
       <c r="M9"/>
     </row>

</xml_diff>

<commit_message>
Generar documentación Gastos Alumnos DUAL
</commit_message>
<xml_diff>
--- a/public/Anexo 6-Gastos_FCT_2DAW.xlsx
+++ b/public/Anexo 6-Gastos_FCT_2DAW.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t xml:space="preserve">CENTRO DOCENTE: </t>
   </si>
@@ -49,7 +49,7 @@
     <t>Fecha:</t>
   </si>
   <si>
-    <t>02-03-2020</t>
+    <t>03-03-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Hoja nº: </t>
@@ -110,12 +110,6 @@
   </si>
   <si>
     <t>Importe Gastos kilometraje (1)</t>
-  </si>
-  <si>
-    <t>Roldán Vara, Sergio</t>
-  </si>
-  <si>
-    <t>Torres Gijón, Beatriz</t>
   </si>
   <si>
     <t>(1) Cuantía €/km según Instrucciones de la Viceconsejería de Educación, Universidades e Investigación vigentes</t>
@@ -673,9 +667,7 @@
       <c r="M7"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
+      <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
@@ -685,16 +677,12 @@
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
-      <c r="K8">
-        <v>5047.0</v>
-      </c>
+      <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
+      <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -704,9 +692,7 @@
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
-      <c r="K9">
-        <v>6.0</v>
-      </c>
+      <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
     </row>
@@ -970,23 +956,23 @@
     </row>
     <row r="23" spans="1:26">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23"/>
       <c r="C23">
         <v>0.12</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L23">
         <f>SUM(L8:L22)</f>
@@ -996,7 +982,7 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H24"/>
     </row>
@@ -1005,15 +991,15 @@
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I26" t="s">
         <v>7</v>

</xml_diff>